<commit_message>
Brought WRI edits in line with version 2.1.1
</commit_message>
<xml_diff>
--- a/InputData/elec/DRC/Demand Response Capacity.xlsx
+++ b/InputData/elec/DRC/Demand Response Capacity.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-brazil\InputData\elec\DRC\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,16 +13,17 @@
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
-    <sheet name="Calculations" sheetId="4" r:id="rId2"/>
-    <sheet name="DRC-BDRC" sheetId="5" r:id="rId3"/>
-    <sheet name="DRC-PADRC" sheetId="2" r:id="rId4"/>
+    <sheet name="Brazil-USA" sheetId="6" r:id="rId2"/>
+    <sheet name="Calculations" sheetId="4" r:id="rId3"/>
+    <sheet name="DRC-BDRC" sheetId="5" r:id="rId4"/>
+    <sheet name="DRC-PADRC" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>Year</t>
   </si>
@@ -88,13 +89,34 @@
   </si>
   <si>
     <t>We then scale the potential from 2030 to 2050 by the growth in peak demand (EPS model output).</t>
+  </si>
+  <si>
+    <t>Ratio</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>Brazil</t>
+  </si>
+  <si>
+    <t>Installed Cap (GW)</t>
+  </si>
+  <si>
+    <t>Notes (Brazil):</t>
+  </si>
+  <si>
+    <t>We were not able to find data for the case of Brazil for the case of this variable</t>
+  </si>
+  <si>
+    <t>Thus, we considered the BAU Demand Response Capacity proportionally to the ratio between the Brazilian installed cap and the US installed capacity</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -118,8 +140,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -129,6 +158,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -142,11 +177,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -167,10 +203,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -475,7 +513,7 @@
   <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -573,15 +611,21 @@
       <c r="B20" s="6"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A21" s="6"/>
+      <c r="A21" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="B21" s="6"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A22" s="6"/>
+      <c r="A22" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="B22" s="6"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A23" s="6"/>
+      <c r="A23" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="B23" s="6"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.45">
@@ -622,10 +666,217 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AJ12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="11.796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:36" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:36" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="3" spans="1:36" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="4" spans="1:36" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="14">
+        <f>B2/B3</f>
+        <v>0.15887850467289719</v>
+      </c>
+    </row>
+    <row r="7" spans="1:36" x14ac:dyDescent="0.45">
+      <c r="A7" s="1"/>
+    </row>
+    <row r="8" spans="1:36" x14ac:dyDescent="0.45">
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="8"/>
+      <c r="Q8" s="8"/>
+      <c r="R8" s="8"/>
+      <c r="S8" s="8"/>
+      <c r="T8" s="8"/>
+      <c r="U8" s="8"/>
+      <c r="V8" s="8"/>
+      <c r="W8" s="8"/>
+      <c r="X8" s="8"/>
+      <c r="Y8" s="8"/>
+      <c r="Z8" s="8"/>
+      <c r="AA8" s="8"/>
+      <c r="AB8" s="8"/>
+      <c r="AC8" s="8"/>
+      <c r="AD8" s="8"/>
+      <c r="AE8" s="8"/>
+      <c r="AF8" s="8"/>
+      <c r="AG8" s="8"/>
+      <c r="AH8" s="8"/>
+      <c r="AI8" s="8"/>
+      <c r="AJ8" s="8"/>
+    </row>
+    <row r="9" spans="1:36" x14ac:dyDescent="0.45">
+      <c r="A9" s="8"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="8"/>
+      <c r="Q9" s="8"/>
+      <c r="R9" s="8"/>
+      <c r="S9" s="8"/>
+      <c r="T9" s="8"/>
+      <c r="U9" s="8"/>
+      <c r="V9" s="8"/>
+      <c r="W9" s="8"/>
+      <c r="X9" s="8"/>
+      <c r="Y9" s="8"/>
+      <c r="Z9" s="8"/>
+      <c r="AA9" s="8"/>
+      <c r="AB9" s="8"/>
+      <c r="AC9" s="8"/>
+      <c r="AD9" s="8"/>
+      <c r="AE9" s="8"/>
+      <c r="AF9" s="8"/>
+      <c r="AG9" s="8"/>
+      <c r="AH9" s="8"/>
+      <c r="AI9" s="8"/>
+      <c r="AJ9" s="8"/>
+    </row>
+    <row r="10" spans="1:36" x14ac:dyDescent="0.45">
+      <c r="A10" s="1"/>
+    </row>
+    <row r="11" spans="1:36" x14ac:dyDescent="0.45">
+      <c r="A11" s="8"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="8"/>
+      <c r="Q11" s="8"/>
+      <c r="R11" s="8"/>
+      <c r="S11" s="8"/>
+      <c r="T11" s="8"/>
+      <c r="U11" s="8"/>
+      <c r="V11" s="8"/>
+      <c r="W11" s="8"/>
+      <c r="X11" s="8"/>
+      <c r="Y11" s="8"/>
+      <c r="Z11" s="8"/>
+      <c r="AA11" s="8"/>
+      <c r="AB11" s="8"/>
+      <c r="AC11" s="8"/>
+      <c r="AD11" s="8"/>
+      <c r="AE11" s="8"/>
+      <c r="AF11" s="8"/>
+      <c r="AG11" s="8"/>
+      <c r="AH11" s="8"/>
+      <c r="AI11" s="8"/>
+      <c r="AJ11" s="8"/>
+    </row>
+    <row r="12" spans="1:36" x14ac:dyDescent="0.45">
+      <c r="A12" s="8"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="8"/>
+      <c r="Q12" s="8"/>
+      <c r="R12" s="8"/>
+      <c r="S12" s="8"/>
+      <c r="T12" s="8"/>
+      <c r="U12" s="8"/>
+      <c r="V12" s="8"/>
+      <c r="W12" s="8"/>
+      <c r="X12" s="8"/>
+      <c r="Y12" s="8"/>
+      <c r="Z12" s="8"/>
+      <c r="AA12" s="8"/>
+      <c r="AB12" s="8"/>
+      <c r="AC12" s="8"/>
+      <c r="AD12" s="8"/>
+      <c r="AE12" s="8"/>
+      <c r="AF12" s="8"/>
+      <c r="AG12" s="8"/>
+      <c r="AH12" s="8"/>
+      <c r="AI12" s="8"/>
+      <c r="AJ12" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -872,268 +1123,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor theme="3"/>
-  </sheetPr>
-  <dimension ref="A1:AH2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="19.265625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.45">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1">
-        <v>2018</v>
-      </c>
-      <c r="C1">
-        <v>2019</v>
-      </c>
-      <c r="D1">
-        <v>2020</v>
-      </c>
-      <c r="E1">
-        <v>2021</v>
-      </c>
-      <c r="F1">
-        <v>2022</v>
-      </c>
-      <c r="G1">
-        <v>2023</v>
-      </c>
-      <c r="H1">
-        <v>2024</v>
-      </c>
-      <c r="I1">
-        <v>2025</v>
-      </c>
-      <c r="J1">
-        <v>2026</v>
-      </c>
-      <c r="K1">
-        <v>2027</v>
-      </c>
-      <c r="L1">
-        <v>2028</v>
-      </c>
-      <c r="M1">
-        <v>2029</v>
-      </c>
-      <c r="N1">
-        <v>2030</v>
-      </c>
-      <c r="O1">
-        <v>2031</v>
-      </c>
-      <c r="P1">
-        <v>2032</v>
-      </c>
-      <c r="Q1">
-        <v>2033</v>
-      </c>
-      <c r="R1">
-        <v>2034</v>
-      </c>
-      <c r="S1">
-        <v>2035</v>
-      </c>
-      <c r="T1">
-        <v>2036</v>
-      </c>
-      <c r="U1">
-        <v>2037</v>
-      </c>
-      <c r="V1">
-        <v>2038</v>
-      </c>
-      <c r="W1">
-        <v>2039</v>
-      </c>
-      <c r="X1">
-        <v>2040</v>
-      </c>
-      <c r="Y1">
-        <v>2041</v>
-      </c>
-      <c r="Z1">
-        <v>2042</v>
-      </c>
-      <c r="AA1">
-        <v>2043</v>
-      </c>
-      <c r="AB1">
-        <v>2044</v>
-      </c>
-      <c r="AC1">
-        <v>2045</v>
-      </c>
-      <c r="AD1">
-        <v>2046</v>
-      </c>
-      <c r="AE1">
-        <v>2047</v>
-      </c>
-      <c r="AF1">
-        <v>2048</v>
-      </c>
-      <c r="AG1">
-        <v>2049</v>
-      </c>
-      <c r="AH1">
-        <v>2050</v>
-      </c>
-    </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.45">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="8">
-        <f>C2</f>
-        <v>59000</v>
-      </c>
-      <c r="C2" s="8">
-        <f>Calculations!A3</f>
-        <v>59000</v>
-      </c>
-      <c r="D2" s="8">
-        <f>$C$2*(Calculations!D7/Calculations!$C$7)</f>
-        <v>56816.464532194783</v>
-      </c>
-      <c r="E2" s="8">
-        <f>$C$2*(Calculations!E7/Calculations!$C$7)</f>
-        <v>58832.246584697867</v>
-      </c>
-      <c r="F2" s="8">
-        <f>$C$2*(Calculations!F7/Calculations!$C$7)</f>
-        <v>59841.508145388158</v>
-      </c>
-      <c r="G2" s="8">
-        <f>$C$2*(Calculations!G7/Calculations!$C$7)</f>
-        <v>60441.185489060117</v>
-      </c>
-      <c r="H2" s="8">
-        <f>$C$2*(Calculations!H7/Calculations!$C$7)</f>
-        <v>60910.319427441813</v>
-      </c>
-      <c r="I2" s="8">
-        <f>$C$2*(Calculations!I7/Calculations!$C$7)</f>
-        <v>61332.85519490626</v>
-      </c>
-      <c r="J2" s="8">
-        <f>$C$2*(Calculations!J7/Calculations!$C$7)</f>
-        <v>61698.445256440929</v>
-      </c>
-      <c r="K2" s="8">
-        <f>$C$2*(Calculations!K7/Calculations!$C$7)</f>
-        <v>62110.496435448993</v>
-      </c>
-      <c r="L2" s="8">
-        <f>$C$2*(Calculations!L7/Calculations!$C$7)</f>
-        <v>62645.416026890351</v>
-      </c>
-      <c r="M2" s="8">
-        <f>$C$2*(Calculations!M7/Calculations!$C$7)</f>
-        <v>63199.865734083796</v>
-      </c>
-      <c r="N2" s="8">
-        <f>$C$2*(Calculations!N7/Calculations!$C$7)</f>
-        <v>63642.822464685501</v>
-      </c>
-      <c r="O2" s="8">
-        <f>$C$2*(Calculations!O7/Calculations!$C$7)</f>
-        <v>64182.53892666247</v>
-      </c>
-      <c r="P2" s="8">
-        <f>$C$2*(Calculations!P7/Calculations!$C$7)</f>
-        <v>64747.267642146486</v>
-      </c>
-      <c r="Q2" s="8">
-        <f>$C$2*(Calculations!Q7/Calculations!$C$7)</f>
-        <v>65344.752130716464</v>
-      </c>
-      <c r="R2" s="8">
-        <f>$C$2*(Calculations!R7/Calculations!$C$7)</f>
-        <v>66060.171107740272</v>
-      </c>
-      <c r="S2" s="8">
-        <f>$C$2*(Calculations!S7/Calculations!$C$7)</f>
-        <v>66822.325309125197</v>
-      </c>
-      <c r="T2" s="8">
-        <f>$C$2*(Calculations!T7/Calculations!$C$7)</f>
-        <v>67635.668971797189</v>
-      </c>
-      <c r="U2" s="8">
-        <f>$C$2*(Calculations!U7/Calculations!$C$7)</f>
-        <v>68486.017064315238</v>
-      </c>
-      <c r="V2" s="8">
-        <f>$C$2*(Calculations!V7/Calculations!$C$7)</f>
-        <v>69383.305961360224</v>
-      </c>
-      <c r="W2" s="8">
-        <f>$C$2*(Calculations!W7/Calculations!$C$7)</f>
-        <v>70259.077467716954</v>
-      </c>
-      <c r="X2" s="8">
-        <f>$C$2*(Calculations!X7/Calculations!$C$7)</f>
-        <v>71106.067750860064</v>
-      </c>
-      <c r="Y2" s="8">
-        <f>$C$2*(Calculations!Y7/Calculations!$C$7)</f>
-        <v>71921.535741912099</v>
-      </c>
-      <c r="Z2" s="8">
-        <f>$C$2*(Calculations!Z7/Calculations!$C$7)</f>
-        <v>72739.744801841618</v>
-      </c>
-      <c r="AA2" s="8">
-        <f>$C$2*(Calculations!AA7/Calculations!$C$7)</f>
-        <v>73533.284241873771</v>
-      </c>
-      <c r="AB2" s="8">
-        <f>$C$2*(Calculations!AB7/Calculations!$C$7)</f>
-        <v>74349.437500145184</v>
-      </c>
-      <c r="AC2" s="8">
-        <f>$C$2*(Calculations!AC7/Calculations!$C$7)</f>
-        <v>75142.291672957959</v>
-      </c>
-      <c r="AD2" s="8">
-        <f>$C$2*(Calculations!AD7/Calculations!$C$7)</f>
-        <v>75921.440501383317</v>
-      </c>
-      <c r="AE2" s="8">
-        <f>$C$2*(Calculations!AE7/Calculations!$C$7)</f>
-        <v>76666.325968840087</v>
-      </c>
-      <c r="AF2" s="8">
-        <f>$C$2*(Calculations!AF7/Calculations!$C$7)</f>
-        <v>77383.800747522007</v>
-      </c>
-      <c r="AG2" s="8">
-        <f>$C$2*(Calculations!AG7/Calculations!$C$7)</f>
-        <v>78049.880484751062</v>
-      </c>
-      <c r="AH2" s="8">
-        <f>$C$2*(Calculations!AH7/Calculations!$C$7)</f>
-        <v>78745.4267124131</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -1145,7 +1134,269 @@
   <dimension ref="A1:AH2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="19.265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:34" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>2018</v>
+      </c>
+      <c r="C1">
+        <v>2019</v>
+      </c>
+      <c r="D1">
+        <v>2020</v>
+      </c>
+      <c r="E1">
+        <v>2021</v>
+      </c>
+      <c r="F1">
+        <v>2022</v>
+      </c>
+      <c r="G1">
+        <v>2023</v>
+      </c>
+      <c r="H1">
+        <v>2024</v>
+      </c>
+      <c r="I1">
+        <v>2025</v>
+      </c>
+      <c r="J1">
+        <v>2026</v>
+      </c>
+      <c r="K1">
+        <v>2027</v>
+      </c>
+      <c r="L1">
+        <v>2028</v>
+      </c>
+      <c r="M1">
+        <v>2029</v>
+      </c>
+      <c r="N1">
+        <v>2030</v>
+      </c>
+      <c r="O1">
+        <v>2031</v>
+      </c>
+      <c r="P1">
+        <v>2032</v>
+      </c>
+      <c r="Q1">
+        <v>2033</v>
+      </c>
+      <c r="R1">
+        <v>2034</v>
+      </c>
+      <c r="S1">
+        <v>2035</v>
+      </c>
+      <c r="T1">
+        <v>2036</v>
+      </c>
+      <c r="U1">
+        <v>2037</v>
+      </c>
+      <c r="V1">
+        <v>2038</v>
+      </c>
+      <c r="W1">
+        <v>2039</v>
+      </c>
+      <c r="X1">
+        <v>2040</v>
+      </c>
+      <c r="Y1">
+        <v>2041</v>
+      </c>
+      <c r="Z1">
+        <v>2042</v>
+      </c>
+      <c r="AA1">
+        <v>2043</v>
+      </c>
+      <c r="AB1">
+        <v>2044</v>
+      </c>
+      <c r="AC1">
+        <v>2045</v>
+      </c>
+      <c r="AD1">
+        <v>2046</v>
+      </c>
+      <c r="AE1">
+        <v>2047</v>
+      </c>
+      <c r="AF1">
+        <v>2048</v>
+      </c>
+      <c r="AG1">
+        <v>2049</v>
+      </c>
+      <c r="AH1">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.45">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="8">
+        <f>C2*'Brazil-USA'!$B$4</f>
+        <v>1489.3003755786528</v>
+      </c>
+      <c r="C2" s="8">
+        <f>Calculations!A3*'Brazil-USA'!$B$4</f>
+        <v>9373.8317757009336</v>
+      </c>
+      <c r="D2" s="8">
+        <f>$C$2*(Calculations!D7/Calculations!$C$7)</f>
+        <v>9026.9149256758064</v>
+      </c>
+      <c r="E2" s="8">
+        <f>$C$2*(Calculations!E7/Calculations!$C$7)</f>
+        <v>9347.1793639239586</v>
+      </c>
+      <c r="F2" s="8">
+        <f>$C$2*(Calculations!F7/Calculations!$C$7)</f>
+        <v>9507.5293315102663</v>
+      </c>
+      <c r="G2" s="8">
+        <f>$C$2*(Calculations!G7/Calculations!$C$7)</f>
+        <v>9602.8051711590833</v>
+      </c>
+      <c r="H2" s="8">
+        <f>$C$2*(Calculations!H7/Calculations!$C$7)</f>
+        <v>9677.3404697804745</v>
+      </c>
+      <c r="I2" s="8">
+        <f>$C$2*(Calculations!I7/Calculations!$C$7)</f>
+        <v>9744.4723206860399</v>
+      </c>
+      <c r="J2" s="8">
+        <f>$C$2*(Calculations!J7/Calculations!$C$7)</f>
+        <v>9802.5567229859407</v>
+      </c>
+      <c r="K2" s="8">
+        <f>$C$2*(Calculations!K7/Calculations!$C$7)</f>
+        <v>9868.0227981554472</v>
+      </c>
+      <c r="L2" s="8">
+        <f>$C$2*(Calculations!L7/Calculations!$C$7)</f>
+        <v>9953.0100229638865</v>
+      </c>
+      <c r="M2" s="8">
+        <f>$C$2*(Calculations!M7/Calculations!$C$7)</f>
+        <v>10041.100163359106</v>
+      </c>
+      <c r="N2" s="8">
+        <f>$C$2*(Calculations!N7/Calculations!$C$7)</f>
+        <v>10111.476466351902</v>
+      </c>
+      <c r="O2" s="8">
+        <f>$C$2*(Calculations!O7/Calculations!$C$7)</f>
+        <v>10197.225810778149</v>
+      </c>
+      <c r="P2" s="8">
+        <f>$C$2*(Calculations!P7/Calculations!$C$7)</f>
+        <v>10286.949064640095</v>
+      </c>
+      <c r="Q2" s="8">
+        <f>$C$2*(Calculations!Q7/Calculations!$C$7)</f>
+        <v>10381.876506749344</v>
+      </c>
+      <c r="R2" s="8">
+        <f>$C$2*(Calculations!R7/Calculations!$C$7)</f>
+        <v>10495.5412040335</v>
+      </c>
+      <c r="S2" s="8">
+        <f>$C$2*(Calculations!S7/Calculations!$C$7)</f>
+        <v>10616.631123879704</v>
+      </c>
+      <c r="T2" s="8">
+        <f>$C$2*(Calculations!T7/Calculations!$C$7)</f>
+        <v>10745.853948790207</v>
+      </c>
+      <c r="U2" s="8">
+        <f>$C$2*(Calculations!U7/Calculations!$C$7)</f>
+        <v>10880.955982180923</v>
+      </c>
+      <c r="V2" s="8">
+        <f>$C$2*(Calculations!V7/Calculations!$C$7)</f>
+        <v>11023.515900403025</v>
+      </c>
+      <c r="W2" s="8">
+        <f>$C$2*(Calculations!W7/Calculations!$C$7)</f>
+        <v>11162.657167768111</v>
+      </c>
+      <c r="X2" s="8">
+        <f>$C$2*(Calculations!X7/Calculations!$C$7)</f>
+        <v>11297.225717426365</v>
+      </c>
+      <c r="Y2" s="8">
+        <f>$C$2*(Calculations!Y7/Calculations!$C$7)</f>
+        <v>11426.786052453323</v>
+      </c>
+      <c r="Z2" s="8">
+        <f>$C$2*(Calculations!Z7/Calculations!$C$7)</f>
+        <v>11556.781884404743</v>
+      </c>
+      <c r="AA2" s="8">
+        <f>$C$2*(Calculations!AA7/Calculations!$C$7)</f>
+        <v>11682.858244036019</v>
+      </c>
+      <c r="AB2" s="8">
+        <f>$C$2*(Calculations!AB7/Calculations!$C$7)</f>
+        <v>11812.527453294093</v>
+      </c>
+      <c r="AC2" s="8">
+        <f>$C$2*(Calculations!AC7/Calculations!$C$7)</f>
+        <v>11938.494938694254</v>
+      </c>
+      <c r="AD2" s="8">
+        <f>$C$2*(Calculations!AD7/Calculations!$C$7)</f>
+        <v>12062.284939472114</v>
+      </c>
+      <c r="AE2" s="8">
+        <f>$C$2*(Calculations!AE7/Calculations!$C$7)</f>
+        <v>12180.631228694219</v>
+      </c>
+      <c r="AF2" s="8">
+        <f>$C$2*(Calculations!AF7/Calculations!$C$7)</f>
+        <v>12294.622548671719</v>
+      </c>
+      <c r="AG2" s="8">
+        <f>$C$2*(Calculations!AG7/Calculations!$C$7)</f>
+        <v>12400.448301315588</v>
+      </c>
+      <c r="AH2" s="8">
+        <f>$C$2*(Calculations!AH7/Calculations!$C$7)</f>
+        <v>12510.955645897406</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="3"/>
+  </sheetPr>
+  <dimension ref="A1:AH2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1262,136 +1513,136 @@
         <v>1</v>
       </c>
       <c r="B2" s="8">
-        <f>C2</f>
-        <v>59000</v>
+        <f>C2*'Brazil-USA'!$B$4</f>
+        <v>1489.3003755786528</v>
       </c>
       <c r="C2" s="8">
-        <f>Calculations!A3</f>
-        <v>59000</v>
+        <f>Calculations!A3*'Brazil-USA'!$B$4</f>
+        <v>9373.8317757009336</v>
       </c>
       <c r="D2" s="8">
-        <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!D1)</f>
-        <v>71636.363636363298</v>
+        <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!D1)*'Brazil-USA'!$B$4</f>
+        <v>11381.478334749308</v>
       </c>
       <c r="E2" s="8">
-        <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!E1)</f>
-        <v>84272.727272730321</v>
+        <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!E1)*'Brazil-USA'!$B$4</f>
+        <v>13389.124893798275</v>
       </c>
       <c r="F2" s="8">
-        <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!F1)</f>
-        <v>96909.090909093618</v>
+        <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!F1)*'Brazil-USA'!$B$4</f>
+        <v>15396.771452846649</v>
       </c>
       <c r="G2" s="8">
-        <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!G1)</f>
-        <v>109545.45454545692</v>
+        <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!G1)*'Brazil-USA'!$B$4</f>
+        <v>17404.418011895024</v>
       </c>
       <c r="H2" s="8">
-        <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!H1)</f>
-        <v>122181.81818182021</v>
+        <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!H1)*'Brazil-USA'!$B$4</f>
+        <v>19412.064570943396</v>
       </c>
       <c r="I2" s="8">
-        <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!I1)</f>
-        <v>134818.18181818351</v>
+        <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!I1)*'Brazil-USA'!$B$4</f>
+        <v>21419.711129991771</v>
       </c>
       <c r="J2" s="8">
-        <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!J1)</f>
-        <v>147454.54545454681</v>
+        <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!J1)*'Brazil-USA'!$B$4</f>
+        <v>23427.357689040145</v>
       </c>
       <c r="K2" s="8">
-        <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!K1)</f>
-        <v>160090.90909091011</v>
+        <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!K1)*'Brazil-USA'!$B$4</f>
+        <v>25435.00424808852</v>
       </c>
       <c r="L2" s="8">
-        <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!L1)</f>
-        <v>172727.2727272734</v>
+        <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!L1)*'Brazil-USA'!$B$4</f>
+        <v>27442.650807136895</v>
       </c>
       <c r="M2" s="8">
-        <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!M1)</f>
-        <v>185363.6363636367</v>
+        <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!M1)*'Brazil-USA'!$B$4</f>
+        <v>29450.29736618527</v>
       </c>
       <c r="N2" s="8">
-        <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!N1)</f>
-        <v>198000</v>
+        <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!N1)*'Brazil-USA'!$B$4</f>
+        <v>31457.943925233641</v>
       </c>
       <c r="O2" s="8">
         <f>$N$2*(Calculations!O7/Calculations!$N$7)</f>
-        <v>199679.11879663626</v>
+        <v>31724.719808811366</v>
       </c>
       <c r="P2" s="8">
         <f>$N$2*(Calculations!P7/Calculations!$N$7)</f>
-        <v>201436.05353547315</v>
+        <v>32003.858972925638</v>
       </c>
       <c r="Q2" s="8">
         <f>$N$2*(Calculations!Q7/Calculations!$N$7)</f>
-        <v>203294.89517943861</v>
+        <v>32299.188953742578</v>
       </c>
       <c r="R2" s="8">
         <f>$N$2*(Calculations!R7/Calculations!$N$7)</f>
-        <v>205520.64432073908</v>
+        <v>32652.812649089385</v>
       </c>
       <c r="S2" s="8">
         <f>$N$2*(Calculations!S7/Calculations!$N$7)</f>
-        <v>207891.79201705556</v>
+        <v>33029.537049438732</v>
       </c>
       <c r="T2" s="8">
         <f>$N$2*(Calculations!T7/Calculations!$N$7)</f>
-        <v>210422.19590193059</v>
+        <v>33431.563834886168</v>
       </c>
       <c r="U2" s="8">
         <f>$N$2*(Calculations!U7/Calculations!$N$7)</f>
-        <v>213067.72474239013</v>
+        <v>33851.881501127398</v>
       </c>
       <c r="V2" s="8">
         <f>$N$2*(Calculations!V7/Calculations!$N$7)</f>
-        <v>215859.29172095226</v>
+        <v>34295.401488375588</v>
       </c>
       <c r="W2" s="8">
         <f>$N$2*(Calculations!W7/Calculations!$N$7)</f>
-        <v>218583.91566978561</v>
+        <v>34728.285667162192</v>
       </c>
       <c r="X2" s="8">
         <f>$N$2*(Calculations!X7/Calculations!$N$7)</f>
-        <v>221218.99798649768</v>
+        <v>35146.943605331406</v>
       </c>
       <c r="Y2" s="8">
         <f>$N$2*(Calculations!Y7/Calculations!$N$7)</f>
-        <v>223756.01089660072</v>
+        <v>35550.020422824411</v>
       </c>
       <c r="Z2" s="8">
         <f>$N$2*(Calculations!Z7/Calculations!$N$7)</f>
-        <v>226301.55158119151</v>
+        <v>35954.45212037622</v>
       </c>
       <c r="AA2" s="8">
         <f>$N$2*(Calculations!AA7/Calculations!$N$7)</f>
-        <v>228770.34229539265</v>
+        <v>36346.689897398828</v>
       </c>
       <c r="AB2" s="8">
         <f>$N$2*(Calculations!AB7/Calculations!$N$7)</f>
-        <v>231309.4871491176</v>
+        <v>36750.105434906531</v>
       </c>
       <c r="AC2" s="8">
         <f>$N$2*(Calculations!AC7/Calculations!$N$7)</f>
-        <v>233776.14591969681</v>
+        <v>37142.004491914442</v>
       </c>
       <c r="AD2" s="8">
         <f>$N$2*(Calculations!AD7/Calculations!$N$7)</f>
-        <v>236200.16581783726</v>
+        <v>37527.129148628344</v>
       </c>
       <c r="AE2" s="8">
         <f>$N$2*(Calculations!AE7/Calculations!$N$7)</f>
-        <v>238517.58853488098</v>
+        <v>37895.31780460725</v>
       </c>
       <c r="AF2" s="8">
         <f>$N$2*(Calculations!AF7/Calculations!$N$7)</f>
-        <v>240749.73350704726</v>
+        <v>38249.957659998159</v>
       </c>
       <c r="AG2" s="8">
         <f>$N$2*(Calculations!AG7/Calculations!$N$7)</f>
-        <v>242821.98270756842</v>
+        <v>38579.193514286562</v>
       </c>
       <c r="AH2" s="8">
         <f>$N$2*(Calculations!AH7/Calculations!$N$7)</f>
-        <v>244985.90548383276</v>
+        <v>38922.994329207067</v>
       </c>
     </row>
   </sheetData>

</xml_diff>